<commit_message>
Opdateret Tidsregistrering for Thomas
</commit_message>
<xml_diff>
--- a/08-Project-Management/Tidsregistrering/Tidsregistrering (Thomas Borg).xlsx
+++ b/08-Project-Management/Tidsregistrering/Tidsregistrering (Thomas Borg).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Navn</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Full dressed Use Case, Test Cases og mockup</t>
   </si>
   <si>
-    <t>2,30 mins</t>
-  </si>
-  <si>
     <t>System Sekvens Diagram</t>
   </si>
   <si>
@@ -70,6 +67,21 @@
   </si>
   <si>
     <t>Undervisning i OC.</t>
+  </si>
+  <si>
+    <t>Activitets Diagram og Domænemodel for UC-5</t>
+  </si>
+  <si>
+    <t>4,30 hrs?</t>
+  </si>
+  <si>
+    <t>2,30 hrs?</t>
+  </si>
+  <si>
+    <t>Test analyst</t>
+  </si>
+  <si>
+    <t>Udarbejdelse af test til OC-2</t>
   </si>
 </sst>
 </file>
@@ -400,7 +412,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,13 +486,13 @@
         <v>42059</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -488,13 +500,13 @@
         <v>42060</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -502,13 +514,41 @@
         <v>42060</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>42061</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>42062</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidsregistrering for Thomas updated
</commit_message>
<xml_diff>
--- a/08-Project-Management/Tidsregistrering/Tidsregistrering (Thomas Borg).xlsx
+++ b/08-Project-Management/Tidsregistrering/Tidsregistrering (Thomas Borg).xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Navn</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Udarbejdelse af test til OC-2</t>
+  </si>
+  <si>
+    <t>Udarbejdelse af AD + Dataordbog for UC 6</t>
+  </si>
+  <si>
+    <t>5 hrs?</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +557,20 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>42069</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>